<commit_message>
get team from excel file implemented
</commit_message>
<xml_diff>
--- a/team_data/Mumbai_India/Mumbai_India.xlsx
+++ b/team_data/Mumbai_India/Mumbai_India.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\2nd Trimester\CM1601 [PRO] Programming Fundamentals\CW\coursework\team_data\Mumbai_India\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B2537B-312A-4629-924E-2B8E2A068EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5143" yWindow="1071" windowWidth="7963" windowHeight="6429" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -73,8 +79,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +143,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -183,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +229,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,6 +281,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,14 +474,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -471,7 +523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -491,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -511,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -531,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -551,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -571,7 +623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -591,7 +643,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -611,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -631,7 +683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -651,7 +703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
get batting team and bowling team implemented
</commit_message>
<xml_diff>
--- a/team_data/Mumbai_India/Mumbai_India.xlsx
+++ b/team_data/Mumbai_India/Mumbai_India.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\2nd Trimester\CM1601 [PRO] Programming Fundamentals\CW\coursework\team_data\Mumbai_India\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B2537B-312A-4629-924E-2B8E2A068EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7408533E-E6F3-4E4A-B36C-727515E32B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5143" yWindow="1071" windowWidth="7963" windowHeight="6429" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="446" windowWidth="7963" windowHeight="6428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -508,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -528,7 +528,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -568,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -588,7 +588,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -688,7 +688,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -708,7 +708,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>0</v>

</xml_diff>